<commit_message>
mengubah password menjadi generatestring
</commit_message>
<xml_diff>
--- a/assets/uploads/sampleformat.xlsx
+++ b/assets/uploads/sampleformat.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="32">
   <si>
     <t>First Name</t>
   </si>
@@ -103,9 +103,6 @@
   </si>
   <si>
     <t>Email*</t>
-  </si>
-  <si>
-    <t>Password*</t>
   </si>
   <si>
     <t>First Name*</t>
@@ -454,18 +451,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -485,52 +479,43 @@
         <v>29</v>
       </c>
       <c r="G1" t="s">
-        <v>30</v>
-      </c>
-      <c r="H1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2">
+        <v>2</v>
+      </c>
+      <c r="F2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B3" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C2">
-        <v>123123213</v>
-      </c>
-      <c r="D2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F2">
-        <v>2</v>
-      </c>
-      <c r="G2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B3" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C3">
-        <v>12312312</v>
+      <c r="C3" t="s">
+        <v>23</v>
       </c>
       <c r="D3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E3" t="s">
         <v>24</v>
       </c>
+      <c r="E3">
+        <v>3</v>
+      </c>
       <c r="F3">
-        <v>3</v>
-      </c>
-      <c r="G3">
         <v>4</v>
       </c>
     </row>

</xml_diff>